<commit_message>
feat: add new project for interface, add new forms for a basic card display.
</commit_message>
<xml_diff>
--- a/VadersLittleHelper.Backend/db/ComponentDB.xlsx
+++ b/VadersLittleHelper.Backend/db/ComponentDB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5295" windowHeight="5790"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5295" windowHeight="5790" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ShipDB" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="649">
   <si>
     <t>Ship</t>
   </si>
@@ -1937,6 +1937,42 @@
   </si>
   <si>
     <t>S0019</t>
+  </si>
+  <si>
+    <t>U0100</t>
+  </si>
+  <si>
+    <t>U0101</t>
+  </si>
+  <si>
+    <t>U0102</t>
+  </si>
+  <si>
+    <t>U0103</t>
+  </si>
+  <si>
+    <t>U0104</t>
+  </si>
+  <si>
+    <t>U0105</t>
+  </si>
+  <si>
+    <t>U0106</t>
+  </si>
+  <si>
+    <t>U0107</t>
+  </si>
+  <si>
+    <t>U0108</t>
+  </si>
+  <si>
+    <t>U0109</t>
+  </si>
+  <si>
+    <t>U0110</t>
+  </si>
+  <si>
+    <t>U0111</t>
   </si>
 </sst>
 </file>
@@ -2323,7 +2359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -6524,9 +6560,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A97" sqref="A97:A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9138,6 +9174,9 @@
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>637</v>
+      </c>
       <c r="B101" s="5" t="s">
         <v>351</v>
       </c>
@@ -9161,6 +9200,9 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>638</v>
+      </c>
       <c r="B102" s="5" t="s">
         <v>353</v>
       </c>
@@ -9184,6 +9226,9 @@
       </c>
     </row>
     <row r="103" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>639</v>
+      </c>
       <c r="B103" s="5" t="s">
         <v>355</v>
       </c>
@@ -9207,6 +9252,9 @@
       </c>
     </row>
     <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>640</v>
+      </c>
       <c r="B104" s="5" t="s">
         <v>357</v>
       </c>
@@ -9230,6 +9278,9 @@
       </c>
     </row>
     <row r="105" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>641</v>
+      </c>
       <c r="B105" s="5" t="s">
         <v>359</v>
       </c>
@@ -9253,6 +9304,9 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>642</v>
+      </c>
       <c r="B106" s="5" t="s">
         <v>361</v>
       </c>
@@ -9276,6 +9330,9 @@
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>643</v>
+      </c>
       <c r="B107" s="5" t="s">
         <v>363</v>
       </c>
@@ -9299,6 +9356,9 @@
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>644</v>
+      </c>
       <c r="B108" s="5" t="s">
         <v>365</v>
       </c>
@@ -9322,6 +9382,9 @@
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>645</v>
+      </c>
       <c r="B109" s="5" t="s">
         <v>367</v>
       </c>
@@ -9345,6 +9408,9 @@
       </c>
     </row>
     <row r="110" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>646</v>
+      </c>
       <c r="B110" s="5" t="s">
         <v>369</v>
       </c>
@@ -9368,6 +9434,9 @@
       </c>
     </row>
     <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>647</v>
+      </c>
       <c r="B111" s="5" t="s">
         <v>371</v>
       </c>
@@ -9391,6 +9460,9 @@
       </c>
     </row>
     <row r="112" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>648</v>
+      </c>
       <c r="B112" s="5" t="s">
         <v>373</v>
       </c>

</xml_diff>

<commit_message>
updated card database to include recent acquisitions
</commit_message>
<xml_diff>
--- a/VadersLittleHelper.Backend/db/ComponentDB.xlsx
+++ b/VadersLittleHelper.Backend/db/ComponentDB.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="741">
   <si>
     <t>Ship</t>
   </si>
@@ -1973,6 +1973,282 @@
   </si>
   <si>
     <t>U0111</t>
+  </si>
+  <si>
+    <t>Tycho Celchu</t>
+  </si>
+  <si>
+    <t>Arvel Crynyd</t>
+  </si>
+  <si>
+    <t>You may declare an enemy ship inside your firing arc that you are touching as the target of your attack.</t>
+  </si>
+  <si>
+    <t>You may perform actions even while you have stress tokens.</t>
+  </si>
+  <si>
+    <t>Concussion Missiles</t>
+  </si>
+  <si>
+    <t>FP: 4, RNG: 2-3 ATTACK (TARGET LOCK): Spend the target lock and discard this card to perfrorm this attack. You may change one of your blank results for a HIT result.</t>
+  </si>
+  <si>
+    <t>Cluster Missiles</t>
+  </si>
+  <si>
+    <t>FP: 3, RNG: 1-2 ATTACK (TARGET LOCK): Spend your target lock and discard this card to perform this attack TWICE.</t>
+  </si>
+  <si>
+    <t>Push The Limit</t>
+  </si>
+  <si>
+    <t>Once per round, after you perform an action, you may perform 1 free action shown in your action bar. Then receive 1 stress token.</t>
+  </si>
+  <si>
+    <t>Deadeye</t>
+  </si>
+  <si>
+    <t>You may treat the 'ATTACK (TARGET LOCK)' header as 'ATTACK (FOCUS)'. When an attack instructs you to spend a target lock, you may spend a focus token instead.</t>
+  </si>
+  <si>
+    <t>Plasma Torpedoes</t>
+  </si>
+  <si>
+    <t>FP: 4, RNG: 2-3 ATTACK (TARGET LOCK): Spend your target lock and discard this card ot perform this attack. If this attack hits, After dealing damage, remove 1 shield token from the defender.</t>
+  </si>
+  <si>
+    <t>Twin Laser Turret</t>
+  </si>
+  <si>
+    <t>FP: 3, RNG: 2-3 ATTACK: Perform this attack TWICE (even against a ship outside your firing arc). Each time this attack hits, the defender suffers 1 damage. Then cancel ALL dice results.</t>
+  </si>
+  <si>
+    <t>Adv. Homing Missiles</t>
+  </si>
+  <si>
+    <t>FP: 3, RNG 2 ATTACK (TARGET LOCK): Discard this card to perfrom this attack. If this attack hits, deal 1 face-up damage card to the defender. Then cancel ALL dice results.</t>
+  </si>
+  <si>
+    <t>Bombardier</t>
+  </si>
+  <si>
+    <t>When dropping a bomb, you may use the [FORWARD 2] template instead of the [FORWARD 1] template.</t>
+  </si>
+  <si>
+    <t>Conner Net</t>
+  </si>
+  <si>
+    <t>ACTION: Discard this card to DROP 1 Conner net token. When a ship's base or maneuver template overlaps this token, this token DETONATES.</t>
+  </si>
+  <si>
+    <t>Extra Munitions</t>
+  </si>
+  <si>
+    <t>When you equip this card, place 1 ordnance token on each equipped TORPEDO, MISSILE and BOMB Upgrade card. When you are instructed to discard an upgrade card, you may discard 1 ordnance token on that card instead.</t>
+  </si>
+  <si>
+    <t>Ion Bombs</t>
+  </si>
+  <si>
+    <t>When you reveal your maneuver dial, you may discard this card to DROP 1 ion bomb token. This token detonates at the end of the activation phase.</t>
+  </si>
+  <si>
+    <t>Advanced SLAM</t>
+  </si>
+  <si>
+    <t>After performing a SLAM action, if you did not overlap an obstacle or another ship, you may perform a free action</t>
+  </si>
+  <si>
+    <t>K-Wing</t>
+  </si>
+  <si>
+    <t>Miranda Doni</t>
+  </si>
+  <si>
+    <t>Once per round when attacking, you may either spend 1 shield to roll 1 additional attack die OR roll 1 fewer attack die to recover 1 shield.</t>
+  </si>
+  <si>
+    <t>Esege Tuketu</t>
+  </si>
+  <si>
+    <t>When another friendly ship at Range 1-2 is attacking, it may treat your focus tokens as its own.</t>
+  </si>
+  <si>
+    <t>Guardian Squadron Pilot</t>
+  </si>
+  <si>
+    <t>Warden Squadron Pilot</t>
+  </si>
+  <si>
+    <t>Scurrg H-6 Bomber</t>
+  </si>
+  <si>
+    <t>S0020</t>
+  </si>
+  <si>
+    <t>S0021</t>
+  </si>
+  <si>
+    <t>Captain Nym</t>
+  </si>
+  <si>
+    <t>Once per round, you may prevent a friendly bomb from detonating.</t>
+  </si>
+  <si>
+    <t>You may ignore friendly bombs. When a friendly ship is defending, if the attacker measures range through a friendly bomb token, the defender may add 1 EVADE result.</t>
+  </si>
+  <si>
+    <t>Sol Sixxa</t>
+  </si>
+  <si>
+    <t>When dropping a bomb, you may use the [TURN 1] template instead of the [FORWARD 1] template.</t>
+  </si>
+  <si>
+    <t>Lok Revenant</t>
+  </si>
+  <si>
+    <t>Karthakk Pirate</t>
+  </si>
+  <si>
+    <t>P0096</t>
+  </si>
+  <si>
+    <t>P0097</t>
+  </si>
+  <si>
+    <t>P0098</t>
+  </si>
+  <si>
+    <t>P0099</t>
+  </si>
+  <si>
+    <t>P0100</t>
+  </si>
+  <si>
+    <t>P0101</t>
+  </si>
+  <si>
+    <t>P0102</t>
+  </si>
+  <si>
+    <t>P0103</t>
+  </si>
+  <si>
+    <t>P0104</t>
+  </si>
+  <si>
+    <t>P0105</t>
+  </si>
+  <si>
+    <t>P0106</t>
+  </si>
+  <si>
+    <t>Lightning Reflexes</t>
+  </si>
+  <si>
+    <t>SMALL SHIP ONLY. After you execute a white or green maneuveron your dial, you may discard this card to rotate your ship 180 degrees. Then receive 1 stress token AFTER the 'check pilot stress' step.</t>
+  </si>
+  <si>
+    <t>Minefield Mapper</t>
+  </si>
+  <si>
+    <t>During setup, after the 'place forces' step, you may discard any number of equipped BOMB upgrade cards. Place all corresponding bomb tokens in the play area beyond Range 3 of enemy ships.</t>
+  </si>
+  <si>
+    <t>Synced Turret</t>
+  </si>
+  <si>
+    <t>FP: 3, RNG 1-2 ATTACK (TARGET LOCK): Attack 1 ship (even a ship outside yoru firing arc). If the defender is inside your primary firing arc, you may reroll a number of attack dice up to your primary weapoon value.</t>
+  </si>
+  <si>
+    <t>Cruise Missiles</t>
+  </si>
+  <si>
+    <t>FP: 1, RNG: 2-3 ATTACK (TARGET LOCK): Discard this card to perform this attack. You may roll additional attack dice equal to the speed of the maneuver you executed this round, to a maximum of 4 additional dice.</t>
+  </si>
+  <si>
+    <t>Cad Bane</t>
+  </si>
+  <si>
+    <t>SCUM ONLY. Your upgrade bar gains the BOMB icon. Once per round, when an enemy ship rolls attack dice due to a friendly bomb detonating, you may choose any number of FOCUS and BLANK results. It must reroll those results.</t>
+  </si>
+  <si>
+    <t>Bomblet Generator</t>
+  </si>
+  <si>
+    <t>When you reveal your maneuver, you may DROP 1 bomblet token. This token detonates at the end of the activation phase. (REQUIRES 2xBOMB SLOTS)</t>
+  </si>
+  <si>
+    <t>R4-E1</t>
+  </si>
+  <si>
+    <t>You can perform actions on you TORPEDO and BOMB Upgrade cards even if you are stressed. After you perform an action in this way, you may discard this card to remove 1 stress token from your ship.</t>
+  </si>
+  <si>
+    <t>Havoc</t>
+  </si>
+  <si>
+    <t>SCURRG H-6 BOMBER ONLY. Your upgrade bar gains the SYSTEM and SALVAGED ASTROMECH upgrade icons, and loses the CREW  upgrade icon. You cannot equip non-unique SALVAGED ASTROMECH Upgrade cards.</t>
+  </si>
+  <si>
+    <t>U0112</t>
+  </si>
+  <si>
+    <t>U0113</t>
+  </si>
+  <si>
+    <t>U0114</t>
+  </si>
+  <si>
+    <t>U0115</t>
+  </si>
+  <si>
+    <t>U0116</t>
+  </si>
+  <si>
+    <t>U0117</t>
+  </si>
+  <si>
+    <t>U0118</t>
+  </si>
+  <si>
+    <t>U0119</t>
+  </si>
+  <si>
+    <t>U0120</t>
+  </si>
+  <si>
+    <t>U0121</t>
+  </si>
+  <si>
+    <t>U0122</t>
+  </si>
+  <si>
+    <t>U0123</t>
+  </si>
+  <si>
+    <t>U0124</t>
+  </si>
+  <si>
+    <t>U0125</t>
+  </si>
+  <si>
+    <t>U0126</t>
+  </si>
+  <si>
+    <t>U0127</t>
+  </si>
+  <si>
+    <t>U0128</t>
+  </si>
+  <si>
+    <t>U0129</t>
+  </si>
+  <si>
+    <t>U0130</t>
+  </si>
+  <si>
+    <t>U0131</t>
   </si>
 </sst>
 </file>
@@ -2357,10 +2633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2497,7 +2773,7 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2586,6 +2862,28 @@
       </c>
       <c r="C20">
         <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>685</v>
+      </c>
+      <c r="B21" t="s">
+        <v>677</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>686</v>
+      </c>
+      <c r="B22" t="s">
+        <v>684</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2596,11 +2894,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:M107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4702,7 +5000,7 @@
         <v>2</v>
       </c>
       <c r="M51" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -4743,7 +5041,7 @@
         <v>2</v>
       </c>
       <c r="M52" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -6547,6 +6845,457 @@
         <v>1</v>
       </c>
       <c r="M96" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="D97" s="9">
+        <v>26</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H97" s="5">
+        <v>8</v>
+      </c>
+      <c r="I97" s="5">
+        <v>2</v>
+      </c>
+      <c r="J97" s="5">
+        <v>3</v>
+      </c>
+      <c r="K97" s="5">
+        <v>2</v>
+      </c>
+      <c r="L97" s="5">
+        <v>2</v>
+      </c>
+      <c r="M97" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="D98" s="9">
+        <v>23</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H98" s="5">
+        <v>6</v>
+      </c>
+      <c r="I98" s="5">
+        <v>2</v>
+      </c>
+      <c r="J98" s="5">
+        <v>3</v>
+      </c>
+      <c r="K98" s="5">
+        <v>2</v>
+      </c>
+      <c r="L98" s="5">
+        <v>2</v>
+      </c>
+      <c r="M98" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>679</v>
+      </c>
+      <c r="D99" s="9">
+        <v>29</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H99" s="5">
+        <v>8</v>
+      </c>
+      <c r="I99" s="5">
+        <v>2</v>
+      </c>
+      <c r="J99" s="5">
+        <v>1</v>
+      </c>
+      <c r="K99" s="5">
+        <v>5</v>
+      </c>
+      <c r="L99" s="5">
+        <v>4</v>
+      </c>
+      <c r="M99" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>681</v>
+      </c>
+      <c r="D100" s="9">
+        <v>28</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H100" s="5">
+        <v>6</v>
+      </c>
+      <c r="I100" s="5">
+        <v>2</v>
+      </c>
+      <c r="J100" s="5">
+        <v>1</v>
+      </c>
+      <c r="K100" s="5">
+        <v>5</v>
+      </c>
+      <c r="L100" s="5">
+        <v>4</v>
+      </c>
+      <c r="M100" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="D101" s="9">
+        <v>25</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H101" s="5">
+        <v>4</v>
+      </c>
+      <c r="I101" s="5">
+        <v>2</v>
+      </c>
+      <c r="J101" s="5">
+        <v>1</v>
+      </c>
+      <c r="K101" s="5">
+        <v>5</v>
+      </c>
+      <c r="L101" s="5">
+        <v>4</v>
+      </c>
+      <c r="M101" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>683</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="D102" s="9">
+        <v>23</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H102" s="5">
+        <v>2</v>
+      </c>
+      <c r="I102" s="5">
+        <v>2</v>
+      </c>
+      <c r="J102" s="5">
+        <v>1</v>
+      </c>
+      <c r="K102" s="5">
+        <v>5</v>
+      </c>
+      <c r="L102" s="5">
+        <v>4</v>
+      </c>
+      <c r="M102" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>688</v>
+      </c>
+      <c r="D103" s="9">
+        <v>30</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H103" s="5">
+        <v>8</v>
+      </c>
+      <c r="I103" s="5">
+        <v>3</v>
+      </c>
+      <c r="J103" s="5">
+        <v>1</v>
+      </c>
+      <c r="K103" s="5">
+        <v>5</v>
+      </c>
+      <c r="L103" s="5">
+        <v>5</v>
+      </c>
+      <c r="M103" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>689</v>
+      </c>
+      <c r="D104" s="9">
+        <v>30</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H104" s="5">
+        <v>8</v>
+      </c>
+      <c r="I104" s="5">
+        <v>3</v>
+      </c>
+      <c r="J104" s="5">
+        <v>1</v>
+      </c>
+      <c r="K104" s="5">
+        <v>5</v>
+      </c>
+      <c r="L104" s="5">
+        <v>5</v>
+      </c>
+      <c r="M104" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>691</v>
+      </c>
+      <c r="D105" s="9">
+        <v>28</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="G105" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H105" s="5">
+        <v>6</v>
+      </c>
+      <c r="I105" s="5">
+        <v>3</v>
+      </c>
+      <c r="J105" s="5">
+        <v>1</v>
+      </c>
+      <c r="K105" s="5">
+        <v>5</v>
+      </c>
+      <c r="L105" s="5">
+        <v>5</v>
+      </c>
+      <c r="M105" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="D106" s="9">
+        <v>26</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H106" s="5">
+        <v>3</v>
+      </c>
+      <c r="I106" s="5">
+        <v>3</v>
+      </c>
+      <c r="J106" s="5">
+        <v>1</v>
+      </c>
+      <c r="K106" s="5">
+        <v>5</v>
+      </c>
+      <c r="L106" s="5">
+        <v>5</v>
+      </c>
+      <c r="M106" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="D107" s="9">
+        <v>24</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H107" s="5">
+        <v>1</v>
+      </c>
+      <c r="I107" s="5">
+        <v>3</v>
+      </c>
+      <c r="J107" s="5">
+        <v>1</v>
+      </c>
+      <c r="K107" s="5">
+        <v>5</v>
+      </c>
+      <c r="L107" s="5">
+        <v>5</v>
+      </c>
+      <c r="M107" s="5">
         <v>1</v>
       </c>
     </row>
@@ -6558,11 +7307,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A97" sqref="A97:A112"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A110" sqref="A110:A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8338,7 +9087,7 @@
         <v>251</v>
       </c>
       <c r="H68" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -8728,7 +9477,7 @@
         <v>246</v>
       </c>
       <c r="H83" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -9482,6 +10231,526 @@
         <v>18</v>
       </c>
       <c r="H112" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="D113" s="5">
+        <v>4</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G113" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="H113" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="D114" s="5">
+        <v>4</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="H114" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="D115" s="5">
+        <v>3</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G115" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H115" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="D116" s="5">
+        <v>1</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H116" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>661</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="D117" s="5">
+        <v>3</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G117" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="H117" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="D118" s="5">
+        <v>6</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G118" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H118" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="D119" s="5">
+        <v>3</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G119" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="H119" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="D120" s="5">
+        <v>1</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G120" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H120" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="D121" s="5">
+        <v>4</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G121" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="H121" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="D122" s="5">
+        <v>2</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G122" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="H122" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="D123" s="5">
+        <v>2</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G123" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="H123" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="D124" s="5">
+        <v>2</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G124" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H124" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="D125" s="5">
+        <v>1</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G125" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H125" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>734</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="D126" s="5">
+        <v>0</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G126" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H126" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="D127" s="5">
+        <v>4</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G127" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H127" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="D128" s="5">
+        <v>3</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="H128" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="D129" s="5">
+        <v>2</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G129" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H129" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="D130" s="5">
+        <v>3</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G130" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="H130" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="D131" s="5">
+        <v>1</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G131" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H131" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>740</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="D132" s="5">
+        <v>0</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H132" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>